<commit_message>
set up kmeans0 experiments
</commit_message>
<xml_diff>
--- a/revision/complete_comparison_fcps/results_summary_nov27_explore.xlsx
+++ b/revision/complete_comparison_fcps/results_summary_nov27_explore.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollywiberg/git/Optimal_Clustering_Trees/revision/complete_comparison_fcps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DA476A-52F9-0942-9A28-1832F06BE0B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC320BB-4C66-E34A-9DAE-002C224CBE1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="460" windowWidth="22660" windowHeight="16540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14300" yWindow="460" windowWidth="23900" windowHeight="16500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="method comparison" sheetId="6" r:id="rId1"/>
     <sheet name="score tables" sheetId="5" r:id="rId2"/>
-    <sheet name="runtime tables" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId3"/>
+    <sheet name="runtime tables" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="79">
   <si>
     <t>Atom</t>
   </si>
@@ -372,6 +373,57 @@
   </si>
   <si>
     <t>Std. Dev Score</t>
+  </si>
+  <si>
+    <t>(N,P)</t>
+  </si>
+  <si>
+    <t>(800,2)</t>
+  </si>
+  <si>
+    <t>(1000,2)</t>
+  </si>
+  <si>
+    <t>(4096,2)</t>
+  </si>
+  <si>
+    <t>(212,3)</t>
+  </si>
+  <si>
+    <t>(400,2)</t>
+  </si>
+  <si>
+    <t>(770,2)</t>
+  </si>
+  <si>
+    <t>(400,3)</t>
+  </si>
+  <si>
+    <t>(1070,2)</t>
+  </si>
+  <si>
+    <t>(1000@2)</t>
+  </si>
+  <si>
+    <t>(4096@2)</t>
+  </si>
+  <si>
+    <t>(212@3)</t>
+  </si>
+  <si>
+    <t>(400@2)</t>
+  </si>
+  <si>
+    <t>(770@2)</t>
+  </si>
+  <si>
+    <t>(400@3)</t>
+  </si>
+  <si>
+    <t>(800@2)</t>
+  </si>
+  <si>
+    <t>(1070@2)</t>
   </si>
 </sst>
 </file>
@@ -1218,7 +1270,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
@@ -1280,28 +1332,22 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1313,16 +1359,22 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="38" xfId="43" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1349,6 +1401,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1396,7 +1450,17 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1414,6 +1478,36 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1808,43 +1902,43 @@
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="50" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="51" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="47"/>
-      <c r="C4" s="61"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="53"/>
+      <c r="E4" s="51"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="47"/>
-      <c r="C5" s="61"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="53"/>
+      <c r="E5" s="51"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="56" t="s">
+      <c r="D6" s="54" t="s">
         <v>38</v>
       </c>
       <c r="E6" s="44" t="s">
@@ -1852,124 +1946,115 @@
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="47"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="57"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="55"/>
       <c r="E7" s="45" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="56" t="s">
         <v>41</v>
       </c>
       <c r="D8" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="52"/>
+      <c r="E8" s="47"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="47"/>
-      <c r="C9" s="60"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="57"/>
       <c r="D9" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="58"/>
+      <c r="E9" s="48"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="52" t="s">
+      <c r="E10" s="47" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="47"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="58"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="48"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="56" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="52" t="s">
+      <c r="E12" s="47" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="47"/>
-      <c r="C13" s="60"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="57"/>
       <c r="D13" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="58"/>
+      <c r="E13" s="48"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="52" t="s">
         <v>52</v>
       </c>
       <c r="D14" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="E14" s="47" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="47"/>
-      <c r="C15" s="50"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="59"/>
       <c r="D15" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="53"/>
+      <c r="E15" s="51"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="47"/>
-      <c r="C16" s="50"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="59"/>
       <c r="D16" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="53"/>
+      <c r="E16" s="51"/>
     </row>
     <row r="17" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="48"/>
-      <c r="C17" s="51"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="60"/>
       <c r="D17" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="E17" s="54"/>
+      <c r="E17" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="C14:C17"/>
     <mergeCell ref="E14:E17"/>
@@ -1980,6 +2065,15 @@
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E7" r:id="rId1" xr:uid="{75C52CEA-29A4-1343-9ED4-38E62F47D910}"/>
@@ -1994,8 +2088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCC6E121-DD84-BB4E-8486-6F7A8CD5A779}">
   <dimension ref="B1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="179" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:C33"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2400,31 +2494,31 @@
       </c>
       <c r="C13" s="65"/>
       <c r="D13" s="5">
-        <f>AVERAGE(D3:D11)</f>
+        <f t="shared" ref="D13:J13" si="2">AVERAGE(D3:D11)</f>
         <v>0.4933333333333334</v>
       </c>
       <c r="E13" s="5">
-        <f>AVERAGE(E3:E11)</f>
+        <f t="shared" si="2"/>
         <v>0.27243333333333336</v>
       </c>
       <c r="F13" s="5">
-        <f>AVERAGE(F3:F11)</f>
+        <f t="shared" si="2"/>
         <v>0.49477777777777782</v>
       </c>
       <c r="G13" s="5">
-        <f>AVERAGE(G3:G11)</f>
+        <f t="shared" si="2"/>
         <v>0.52777777777777779</v>
       </c>
       <c r="H13" s="5">
-        <f>AVERAGE(H3:H11)</f>
+        <f t="shared" si="2"/>
         <v>0.5364444444444445</v>
       </c>
       <c r="I13" s="5">
-        <f>AVERAGE(I3:I11)</f>
+        <f t="shared" si="2"/>
         <v>0.45633333333333337</v>
       </c>
       <c r="J13" s="17">
-        <f>AVERAGE(J3:J11)</f>
+        <f t="shared" si="2"/>
         <v>0.40855555555555556</v>
       </c>
       <c r="K13" s="30"/>
@@ -2439,27 +2533,27 @@
         <v>6.2267567802187347E-2</v>
       </c>
       <c r="E14" s="5">
-        <f t="shared" ref="E14:J14" si="2">STDEV(E3:E11)</f>
+        <f t="shared" ref="E14:J14" si="3">STDEV(E3:E11)</f>
         <v>0.25046246225732105</v>
       </c>
       <c r="F14" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.0835910611834233E-2</v>
       </c>
       <c r="G14" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.10075189548809672</v>
       </c>
       <c r="H14" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.0083448966931365E-2</v>
       </c>
       <c r="I14" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.3730929737797504E-2</v>
       </c>
       <c r="J14" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.15331675635030179</v>
       </c>
       <c r="K14" s="30"/>
@@ -2505,31 +2599,31 @@
       </c>
       <c r="C16" s="67"/>
       <c r="D16" s="7">
-        <f>($D$13-D13)/D13</f>
+        <f t="shared" ref="D16:J16" si="4">($D$13-D13)/D13</f>
         <v>0</v>
       </c>
       <c r="E16" s="7">
-        <f>($D$13-E13)/E13</f>
+        <f t="shared" si="4"/>
         <v>0.81084057261715414</v>
       </c>
       <c r="F16" s="7">
-        <f>($D$13-F13)/F13</f>
+        <f t="shared" si="4"/>
         <v>-2.919380193128168E-3</v>
       </c>
       <c r="G16" s="7">
-        <f>($D$13-G13)/G13</f>
+        <f t="shared" si="4"/>
         <v>-6.5263157894736731E-2</v>
       </c>
       <c r="H16" s="7">
-        <f>($D$13-H13)/H13</f>
+        <f t="shared" si="4"/>
         <v>-8.0364540182270058E-2</v>
       </c>
       <c r="I16" s="7">
-        <f>($D$13-I13)/I13</f>
+        <f t="shared" si="4"/>
         <v>8.1081081081081141E-2</v>
       </c>
       <c r="J16" s="28">
-        <f>($D$13-J13)/J13</f>
+        <f t="shared" si="4"/>
         <v>0.20750611911884703</v>
       </c>
       <c r="K16" s="31"/>
@@ -2620,7 +2714,7 @@
         <v>0.371</v>
       </c>
       <c r="K20" s="4">
-        <f t="shared" ref="K20:K28" si="3">MAX(D20:I20)</f>
+        <f t="shared" ref="K20:K28" si="5">MAX(D20:I20)</f>
         <v>0.13700000000000001</v>
       </c>
     </row>
@@ -2653,7 +2747,7 @@
         <v>0.26500000000000001</v>
       </c>
       <c r="K21" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.26500000000000001</v>
       </c>
     </row>
@@ -2686,7 +2780,7 @@
         <v>2.5900000000000001E-4</v>
       </c>
       <c r="K22" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
@@ -2719,7 +2813,7 @@
         <v>1.08</v>
       </c>
       <c r="K23" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.08</v>
       </c>
     </row>
@@ -2752,7 +2846,7 @@
         <v>0.11700000000000001</v>
       </c>
       <c r="K24" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.11700000000000001</v>
       </c>
     </row>
@@ -2785,7 +2879,7 @@
         <v>0.253</v>
       </c>
       <c r="K25" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.55000000000000004</v>
       </c>
     </row>
@@ -2818,7 +2912,7 @@
         <v>0.2</v>
       </c>
       <c r="K26" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
     </row>
@@ -2851,7 +2945,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="K27" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
@@ -2884,7 +2978,7 @@
         <v>6.3299999999999995E-2</v>
       </c>
       <c r="K28" s="4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.3299999999999995E-2</v>
       </c>
     </row>
@@ -2894,27 +2988,27 @@
       </c>
       <c r="C29" s="63"/>
       <c r="D29" s="12">
-        <f t="shared" ref="D29:I29" si="4">SUMPRODUCT(--(D20:D28=$K$20:$K$28))</f>
+        <f t="shared" ref="D29:I29" si="6">SUMPRODUCT(--(D20:D28=$K$20:$K$28))</f>
         <v>5</v>
       </c>
       <c r="E29" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="F29" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G29" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="H29" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="I29" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J29" s="12">
@@ -2929,31 +3023,31 @@
       </c>
       <c r="C30" s="65"/>
       <c r="D30" s="5">
-        <f t="shared" ref="D30:J30" si="5">AVERAGE(D20:D28)</f>
+        <f t="shared" ref="D30:J30" si="7">AVERAGE(D20:D28)</f>
         <v>0.16726666666666667</v>
       </c>
       <c r="E30" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.20423333333333332</v>
       </c>
       <c r="F30" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.11315777777777776</v>
       </c>
       <c r="G30" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.23708888888888893</v>
       </c>
       <c r="H30" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.16743111111111111</v>
       </c>
       <c r="I30" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3.9167777777777781E-2</v>
       </c>
       <c r="J30" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.26350655555555558</v>
       </c>
       <c r="K30" s="30"/>
@@ -2968,27 +3062,27 @@
         <v>0.17098788699788064</v>
       </c>
       <c r="E31" s="5">
-        <f t="shared" ref="E31:J31" si="6">STDEV(E20:E28)</f>
+        <f t="shared" ref="E31:J31" si="8">STDEV(E20:E28)</f>
         <v>0.34086803531572163</v>
       </c>
       <c r="F31" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.15281904836912327</v>
       </c>
       <c r="G31" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.35754133832483076</v>
       </c>
       <c r="H31" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.34704513713796814</v>
       </c>
       <c r="I31" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>6.2610511453305068E-2</v>
       </c>
       <c r="J31" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.33006317836404869</v>
       </c>
       <c r="K31" s="30"/>
@@ -3034,31 +3128,31 @@
       </c>
       <c r="C33" s="67"/>
       <c r="D33" s="7">
-        <f t="shared" ref="D33:J33" si="7">($D$30-D30)/D30</f>
+        <f t="shared" ref="D33:J33" si="9">($D$30-D30)/D30</f>
         <v>0</v>
       </c>
       <c r="E33" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-0.18100212175616118</v>
       </c>
       <c r="F33" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.47817207046208865</v>
       </c>
       <c r="G33" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-0.29449807854531829</v>
       </c>
       <c r="H33" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-9.8216181779567954E-4</v>
       </c>
       <c r="I33" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3.2705171484496893</v>
       </c>
       <c r="J33" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-0.36522768356174146</v>
       </c>
       <c r="K33" s="31"/>
@@ -3079,27 +3173,27 @@
     <mergeCell ref="B31:C31"/>
   </mergeCells>
   <conditionalFormatting sqref="D34:I38 D15:J17 H29:J29 D23:I28 H20:I28 D20:G29 D32:J33 D3:I12 J12">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="10" priority="8">
       <formula>AND(D3&lt;&gt;0,D3=$K3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:C28">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="lessThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C11">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="lessThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P11">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>AND(P3&lt;&gt;0,P3=$K3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:I12 K12">
-    <cfRule type="expression" dxfId="2" priority="10">
+    <cfRule type="expression" dxfId="6" priority="10">
       <formula>AND(D12&lt;&gt;0,D12=$K13)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3108,6 +3202,759 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56519113-0F44-D549-9CCF-BB86C7A47199}">
+  <dimension ref="A1:I28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A17:I28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="D3" s="3">
+        <v>-1.2E-2</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="I3" s="23">
+        <v>0.311</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.39</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.496</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.501</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="I4" s="24">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.161</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.433</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.379</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.438</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.434</v>
+      </c>
+      <c r="I5" s="24">
+        <v>0.39800000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.374</v>
+      </c>
+      <c r="I6" s="25">
+        <v>0.70199999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.439</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="I7" s="24">
+        <v>0.439</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="I8" s="24">
+        <v>0.29499999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.504</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.504</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.504</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.504</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.504</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.504</v>
+      </c>
+      <c r="I9" s="25">
+        <v>0.504</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="D10" s="3">
+        <v>4.7300000000000002E-2</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="I10" s="25">
+        <v>0.48599999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2.6599999999999999E-2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="I11" s="26">
+        <v>0.38400000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="70" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="71"/>
+      <c r="C12" s="5">
+        <f t="shared" ref="C12:I12" si="0">AVERAGE(C3:C11)</f>
+        <v>0.4933333333333334</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" si="0"/>
+        <v>0.27243333333333336</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="0"/>
+        <v>0.49477777777777782</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="0"/>
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="0"/>
+        <v>0.5364444444444445</v>
+      </c>
+      <c r="H12" s="5">
+        <f t="shared" si="0"/>
+        <v>0.45633333333333337</v>
+      </c>
+      <c r="I12" s="17">
+        <f t="shared" si="0"/>
+        <v>0.40855555555555556</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="70" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="71"/>
+      <c r="C13" s="5">
+        <f>STDEV(C3:C11)</f>
+        <v>6.2267567802187347E-2</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" ref="D13:I13" si="1">STDEV(D3:D11)</f>
+        <v>0.25046246225732105</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="1"/>
+        <v>8.0835910611834233E-2</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="1"/>
+        <v>0.10075189548809672</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" si="1"/>
+        <v>9.0083448966931365E-2</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="1"/>
+        <v>7.3730929737797504E-2</v>
+      </c>
+      <c r="I13" s="17">
+        <f t="shared" si="1"/>
+        <v>0.15331675635030179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="13">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="D18" s="14">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="E18" s="14">
+        <v>4.7699999999999999E-2</v>
+      </c>
+      <c r="F18" s="14">
+        <v>9.7199999999999995E-2</v>
+      </c>
+      <c r="G18" s="14">
+        <v>5.21E-2</v>
+      </c>
+      <c r="H18" s="16">
+        <v>5.3600000000000002E-2</v>
+      </c>
+      <c r="I18" s="21">
+        <v>0.371</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="15">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="E19" s="5">
+        <v>1.61E-2</v>
+      </c>
+      <c r="F19" s="5">
+        <v>3.73E-2</v>
+      </c>
+      <c r="G19" s="5">
+        <v>3.0300000000000001E-2</v>
+      </c>
+      <c r="H19" s="17">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="I19" s="22">
+        <v>0.26500000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="15">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="D20" s="5">
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="E20" s="5">
+        <v>4.4200000000000003E-3</v>
+      </c>
+      <c r="F20" s="5">
+        <v>1.38E-2</v>
+      </c>
+      <c r="G20" s="5">
+        <v>4.4799999999999996E-3</v>
+      </c>
+      <c r="H20" s="17">
+        <v>1.6199999999999999E-3</v>
+      </c>
+      <c r="I20" s="32">
+        <v>2.5900000000000001E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="15">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1.08</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="F21" s="5">
+        <v>1.08</v>
+      </c>
+      <c r="G21" s="5">
+        <v>1.08</v>
+      </c>
+      <c r="H21" s="17">
+        <v>2.7400000000000001E-2</v>
+      </c>
+      <c r="I21" s="22">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="15">
+        <v>9.6500000000000002E-2</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="F22" s="5">
+        <v>7.0499999999999993E-2</v>
+      </c>
+      <c r="G22" s="5">
+        <v>6.0400000000000002E-2</v>
+      </c>
+      <c r="H22" s="17">
+        <v>3.4799999999999998E-2</v>
+      </c>
+      <c r="I22" s="22">
+        <v>0.11700000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="15">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0.113</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G23" s="5">
+        <v>2.8799999999999999E-2</v>
+      </c>
+      <c r="H23" s="17">
+        <v>1.2E-2</v>
+      </c>
+      <c r="I23" s="32">
+        <v>0.253</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="H24" s="17">
+        <v>0.2</v>
+      </c>
+      <c r="I24" s="22">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="15">
+        <v>4.36E-2</v>
+      </c>
+      <c r="D25" s="5">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="E25" s="5">
+        <v>2.0799999999999999E-2</v>
+      </c>
+      <c r="F25" s="5">
+        <v>4.8599999999999997E-2</v>
+      </c>
+      <c r="G25" s="5">
+        <v>2.4799999999999999E-2</v>
+      </c>
+      <c r="H25" s="17">
+        <v>5.3400000000000001E-3</v>
+      </c>
+      <c r="I25" s="32">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="15">
+        <v>6.3299999999999995E-2</v>
+      </c>
+      <c r="D26" s="5">
+        <v>1.9099999999999999E-2</v>
+      </c>
+      <c r="E26" s="5">
+        <v>1.7399999999999999E-2</v>
+      </c>
+      <c r="F26" s="5">
+        <v>3.6400000000000002E-2</v>
+      </c>
+      <c r="G26" s="5">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="H26" s="17">
+        <v>8.5500000000000003E-3</v>
+      </c>
+      <c r="I26" s="22">
+        <v>6.3299999999999995E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="70" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="71"/>
+      <c r="C27" s="5">
+        <f t="shared" ref="C27:I27" si="2">AVERAGE(C18:C26)</f>
+        <v>0.16726666666666667</v>
+      </c>
+      <c r="D27" s="5">
+        <f t="shared" si="2"/>
+        <v>0.20423333333333332</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" si="2"/>
+        <v>0.11315777777777776</v>
+      </c>
+      <c r="F27" s="5">
+        <f t="shared" si="2"/>
+        <v>0.23708888888888893</v>
+      </c>
+      <c r="G27" s="5">
+        <f t="shared" si="2"/>
+        <v>0.16743111111111111</v>
+      </c>
+      <c r="H27" s="5">
+        <f t="shared" si="2"/>
+        <v>3.9167777777777781E-2</v>
+      </c>
+      <c r="I27" s="17">
+        <f t="shared" si="2"/>
+        <v>0.26350655555555558</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="70" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="71"/>
+      <c r="C28" s="5">
+        <f>STDEV(C18:C26)</f>
+        <v>0.17098788699788064</v>
+      </c>
+      <c r="D28" s="5">
+        <f t="shared" ref="D28:I28" si="3">STDEV(D18:D26)</f>
+        <v>0.34086803531572163</v>
+      </c>
+      <c r="E28" s="5">
+        <f t="shared" si="3"/>
+        <v>0.15281904836912327</v>
+      </c>
+      <c r="F28" s="5">
+        <f t="shared" si="3"/>
+        <v>0.35754133832483076</v>
+      </c>
+      <c r="G28" s="5">
+        <f t="shared" si="3"/>
+        <v>0.34704513713796814</v>
+      </c>
+      <c r="H28" s="5">
+        <f t="shared" si="3"/>
+        <v>6.2610511453305068E-2</v>
+      </c>
+      <c r="I28" s="17">
+        <f t="shared" si="3"/>
+        <v>0.33006317836404869</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B3:B11">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:H11">
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>AND(C3&lt;&gt;0,C3=$J3)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:H26">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>AND(C18&lt;&gt;0,C18=$K18)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:B26">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C697C32-4104-D241-84E3-A0B4F13795AE}">
   <dimension ref="B1:J24"/>
   <sheetViews>
@@ -3742,12 +4589,12 @@
     <mergeCell ref="B14:J14"/>
   </mergeCells>
   <conditionalFormatting sqref="D12:I13 D16:I24">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>AND(D12&lt;&gt;0,D12=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:I11">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>AND(D3&lt;&gt;0,D3=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>